<commit_message>
test: results on EPFL under ER <= 0.01
</commit_message>
<xml_diff>
--- a/ANS-VECBEE/result/epfl-er.xlsx
+++ b/ANS-VECBEE/result/epfl-er.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>er bound = 0.01</t>
   </si>
@@ -40,9 +40,6 @@
     <t>#i/o</t>
   </si>
   <si>
-    <t>delay (from abc)</t>
-  </si>
-  <si>
     <t>error rate</t>
   </si>
   <si>
@@ -89,12 +86,6 @@
   </si>
   <si>
     <t>128/128</t>
-  </si>
-  <si>
-    <t>hyp</t>
-  </si>
-  <si>
-    <t>255/128</t>
   </si>
   <si>
     <t>i2c</t>
@@ -179,10 +170,16 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -332,12 +329,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -637,152 +640,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -795,7 +798,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
@@ -1123,10 +1138,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>
@@ -1177,21 +1192,21 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>9</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>10</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>2594</v>
@@ -1203,28 +1218,28 @@
         <v>1117</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4">
-        <v>2518</v>
-      </c>
-      <c r="G4">
-        <v>207.5</v>
-      </c>
-      <c r="H4" s="4">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2512</v>
+      </c>
+      <c r="G4" s="4">
+        <v>302.6</v>
+      </c>
+      <c r="H4" s="5">
         <v>0</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="9">
         <f t="shared" ref="I4:I10" si="0">F4/B4</f>
-        <v>0.970701619121049</v>
-      </c>
-      <c r="J4" s="6">
+        <v>0.968388589051658</v>
+      </c>
+      <c r="J4" s="10">
         <v>3.84195</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>1802</v>
@@ -1236,28 +1251,28 @@
         <v>857</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5">
         <v>1198</v>
       </c>
       <c r="G5">
-        <v>45.9</v>
-      </c>
-      <c r="H5" s="4">
+        <v>64.5</v>
+      </c>
+      <c r="H5" s="5">
         <v>0.00885</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="9">
         <f t="shared" si="0"/>
         <v>0.664816870144284</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="10">
         <v>99.2991</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>5383</v>
@@ -1269,28 +1284,28 @@
         <v>1927</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6">
-        <v>5126</v>
-      </c>
-      <c r="G6">
-        <v>20.9</v>
-      </c>
-      <c r="H6" s="4">
+        <v>15</v>
+      </c>
+      <c r="F6" s="6">
+        <v>5383</v>
+      </c>
+      <c r="G6" s="6">
+        <v>51.6</v>
+      </c>
+      <c r="H6" s="5">
         <v>0</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="9">
         <f t="shared" si="0"/>
-        <v>0.952257105703139</v>
-      </c>
-      <c r="J6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="10">
         <v>6.89306</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>1093</v>
@@ -1302,28 +1317,28 @@
         <v>441</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7">
-        <v>1034</v>
-      </c>
-      <c r="G7">
-        <v>14.6</v>
-      </c>
-      <c r="H7" s="4">
+        <v>17</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1070</v>
+      </c>
+      <c r="G7" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="H7" s="5">
         <v>0.0099</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="9">
         <f t="shared" si="0"/>
-        <v>0.946020128087832</v>
-      </c>
-      <c r="J7" s="6">
+        <v>0.978956999085087</v>
+      </c>
+      <c r="J7" s="10">
         <v>6.79064</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>195</v>
@@ -1335,28 +1350,28 @@
         <v>87</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8">
         <v>183</v>
       </c>
       <c r="G8">
-        <v>7.2</v>
-      </c>
-      <c r="H8" s="4">
+        <v>11.9</v>
+      </c>
+      <c r="H8" s="5">
         <v>0.00751</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="9">
         <f t="shared" si="0"/>
         <v>0.938461538461538</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="10">
         <v>0.374605</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>995</v>
@@ -1368,28 +1383,28 @@
         <v>433</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9">
         <v>714</v>
       </c>
       <c r="G9">
-        <v>7</v>
-      </c>
-      <c r="H9" s="4">
+        <v>15.5</v>
+      </c>
+      <c r="H9" s="5">
         <v>0.00734</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="9">
         <f t="shared" si="0"/>
         <v>0.717587939698492</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="10">
         <v>6.16086</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <f>47469</f>
@@ -1402,440 +1417,430 @@
         <v>17710</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5">
+        <v>23</v>
+      </c>
+      <c r="F10">
+        <v>10117</v>
+      </c>
+      <c r="G10">
+        <v>1668.2</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.00995508</v>
+      </c>
+      <c r="I10" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="6"/>
+        <v>0.21312856811814</v>
+      </c>
+      <c r="J10" s="10">
+        <v>92930.7</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>1428</v>
+      </c>
+      <c r="C11">
+        <v>31.2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>611</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B11">
-        <f>481912</f>
-        <v>481912</v>
-      </c>
-      <c r="C11">
-        <v>32580</v>
-      </c>
-      <c r="D11" s="2">
-        <v>181271</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="6"/>
+      <c r="F11">
+        <v>1102</v>
+      </c>
+      <c r="G11">
+        <v>31.2</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.00895</v>
+      </c>
+      <c r="I11" s="9">
+        <f t="shared" ref="I11:I22" si="1">F11/B11</f>
+        <v>0.771708683473389</v>
+      </c>
+      <c r="J11" s="10">
+        <v>82.019</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>341</v>
+      </c>
+      <c r="C12">
+        <v>19.5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>147</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B12">
-        <v>1428</v>
-      </c>
-      <c r="C12">
-        <v>31.2</v>
-      </c>
-      <c r="D12" s="1">
-        <v>611</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="F12">
-        <v>1102</v>
-      </c>
-      <c r="G12">
-        <v>17.6</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0.00895</v>
-      </c>
-      <c r="I12" s="5">
-        <f t="shared" ref="I12:I23" si="1">F12/B12</f>
-        <v>0.771708683473389</v>
-      </c>
-      <c r="J12" s="6">
-        <v>82.019</v>
+        <v>256</v>
+      </c>
+      <c r="G12" s="7">
+        <v>18.1</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.00959</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="shared" si="1"/>
+        <v>0.750733137829912</v>
+      </c>
+      <c r="J12" s="10">
+        <v>2.2399</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>69688</v>
+      </c>
+      <c r="C13">
+        <v>651.4</v>
+      </c>
+      <c r="D13" s="1">
+        <v>27468</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B13">
-        <v>341</v>
-      </c>
-      <c r="C13">
-        <v>19.5</v>
-      </c>
-      <c r="D13" s="1">
-        <v>147</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13">
-        <v>255</v>
-      </c>
-      <c r="G13">
-        <v>10.7</v>
-      </c>
-      <c r="H13" s="4">
-        <v>0.00959</v>
-      </c>
-      <c r="I13" s="5">
+      <c r="F13" s="4">
+        <f>61634</f>
+        <v>61634</v>
+      </c>
+      <c r="G13" s="4">
+        <v>632.1</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.00952539</v>
+      </c>
+      <c r="I13" s="9">
         <f t="shared" si="1"/>
-        <v>0.747800586510264</v>
-      </c>
-      <c r="J13" s="6">
-        <v>2.2399</v>
+        <v>0.884427735047641</v>
+      </c>
+      <c r="J13" s="10">
+        <v>42595.9</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>5041</v>
+      </c>
+      <c r="C14">
+        <v>466.9</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2163</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B14">
-        <v>69688</v>
-      </c>
-      <c r="C14">
-        <v>651.4</v>
-      </c>
-      <c r="D14" s="1">
-        <v>27468</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="F14">
-        <v>58159</v>
+        <v>2377</v>
       </c>
       <c r="G14">
-        <v>431.6</v>
-      </c>
-      <c r="H14" s="4">
-        <v>0.00952539</v>
-      </c>
-      <c r="I14" s="5">
+        <v>146.7</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.00869</v>
+      </c>
+      <c r="I14" s="9">
         <f t="shared" si="1"/>
-        <v>0.834562621972219</v>
-      </c>
-      <c r="J14" s="6">
-        <v>42595.9</v>
+        <v>0.471533425907558</v>
+      </c>
+      <c r="J14" s="10">
+        <v>526.586</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>14671</v>
+      </c>
+      <c r="C15">
+        <v>101.9</v>
+      </c>
+      <c r="D15" s="2">
+        <v>6205</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B15">
-        <v>5041</v>
-      </c>
-      <c r="C15">
-        <v>466.9</v>
-      </c>
-      <c r="D15" s="1">
-        <v>2163</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="F15">
-        <v>2377</v>
+        <v>9869</v>
       </c>
       <c r="G15">
-        <v>34.4</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0.00869</v>
-      </c>
-      <c r="I15" s="5">
+        <v>94.5</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.00960156</v>
+      </c>
+      <c r="I15" s="9">
         <f t="shared" si="1"/>
-        <v>0.471533425907558</v>
-      </c>
-      <c r="J15" s="6">
-        <v>526.586</v>
+        <v>0.672687615022834</v>
+      </c>
+      <c r="J15" s="10">
+        <v>43127.4</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16">
-        <v>14671</v>
+        <v>54205</v>
       </c>
       <c r="C16">
-        <v>101.9</v>
+        <v>419.5</v>
       </c>
       <c r="D16" s="2">
-        <v>6205</v>
+        <v>20260</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16">
-        <v>9869</v>
-      </c>
-      <c r="G16">
-        <v>37.4</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0.00960156</v>
-      </c>
-      <c r="I16" s="5">
+        <v>23</v>
+      </c>
+      <c r="F16" s="6">
+        <v>52191</v>
+      </c>
+      <c r="G16" s="8">
+        <v>549.9</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.00937793</v>
+      </c>
+      <c r="I16" s="9">
         <f t="shared" si="1"/>
-        <v>0.672687615022834</v>
-      </c>
-      <c r="J16" s="6">
-        <v>43127.4</v>
+        <v>0.962844756018817</v>
+      </c>
+      <c r="J16" s="10">
+        <v>67837.1</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17">
-        <v>54205</v>
+        <v>741</v>
       </c>
       <c r="C17">
-        <v>419.5</v>
-      </c>
-      <c r="D17" s="2">
-        <v>20260</v>
+        <v>126.8</v>
+      </c>
+      <c r="D17" s="1">
+        <v>351</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F17">
-        <v>51445</v>
+        <v>26</v>
       </c>
       <c r="G17">
-        <v>348.1</v>
-      </c>
-      <c r="H17" s="4">
-        <v>0.00937793</v>
-      </c>
-      <c r="I17" s="5">
+        <v>6.8</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0.00382</v>
+      </c>
+      <c r="I17" s="9">
         <f t="shared" si="1"/>
-        <v>0.949082187990038</v>
-      </c>
-      <c r="J17" s="6">
-        <v>67837.1</v>
+        <v>0.0350877192982456</v>
+      </c>
+      <c r="J17" s="10">
+        <v>134.567</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18">
+        <v>186</v>
+      </c>
+      <c r="C18">
+        <v>13.7</v>
+      </c>
+      <c r="D18" s="1">
+        <v>109</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B18">
-        <v>741</v>
-      </c>
-      <c r="C18">
-        <v>126.8</v>
-      </c>
-      <c r="D18" s="1">
-        <v>351</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="F18">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="G18">
-        <v>5.7</v>
-      </c>
-      <c r="H18" s="4">
-        <v>0.00382</v>
-      </c>
-      <c r="I18" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.00627</v>
+      </c>
+      <c r="I18" s="9">
         <f t="shared" si="1"/>
-        <v>0.0350877192982456</v>
-      </c>
-      <c r="J18" s="6">
-        <v>134.567</v>
+        <v>0.021505376344086</v>
+      </c>
+      <c r="J18" s="10">
+        <v>17.1458</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19">
+        <v>13552</v>
+      </c>
+      <c r="C19">
+        <v>272.9</v>
+      </c>
+      <c r="D19" s="1">
+        <v>5534</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B19">
-        <v>186</v>
-      </c>
-      <c r="C19">
-        <v>13.7</v>
-      </c>
-      <c r="D19" s="1">
-        <v>109</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19">
-        <v>4</v>
-      </c>
-      <c r="G19">
-        <v>1.4</v>
-      </c>
-      <c r="H19" s="4">
-        <v>0.00627</v>
-      </c>
-      <c r="I19" s="5">
+      <c r="F19" s="4">
+        <v>12159</v>
+      </c>
+      <c r="G19" s="4">
+        <v>267.5</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0.00979</v>
+      </c>
+      <c r="I19" s="9">
         <f t="shared" si="1"/>
-        <v>0.021505376344086</v>
-      </c>
-      <c r="J19" s="6">
-        <v>17.1458</v>
+        <v>0.897210743801653</v>
+      </c>
+      <c r="J19" s="10">
+        <v>319.22</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20">
+        <v>43859</v>
+      </c>
+      <c r="C20">
+        <v>7304</v>
+      </c>
+      <c r="D20" s="2">
+        <v>16584</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B20">
-        <v>13552</v>
-      </c>
-      <c r="C20">
-        <v>272.9</v>
-      </c>
-      <c r="D20" s="1">
-        <v>5534</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="F20">
-        <v>11391</v>
+        <v>30649</v>
       </c>
       <c r="G20">
-        <v>183.4</v>
-      </c>
-      <c r="H20" s="4">
-        <v>0.00979</v>
-      </c>
-      <c r="I20" s="5">
+        <v>6930</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.00773047</v>
+      </c>
+      <c r="I20" s="9">
         <f t="shared" si="1"/>
-        <v>0.840540141676505</v>
-      </c>
-      <c r="J20" s="6">
-        <v>319.22</v>
+        <v>0.698807542351627</v>
+      </c>
+      <c r="J20" s="10">
+        <v>75064.5</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21">
+        <v>37672</v>
+      </c>
+      <c r="C21">
+        <v>355.5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>14967</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B21">
-        <v>43859</v>
-      </c>
-      <c r="C21">
-        <v>7304</v>
-      </c>
-      <c r="D21" s="2">
-        <v>16584</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21">
-        <v>30649</v>
-      </c>
-      <c r="G21">
-        <v>3687.22</v>
-      </c>
-      <c r="H21" s="4">
-        <v>0.00773047</v>
-      </c>
-      <c r="I21" s="5">
+      <c r="F21" s="8">
+        <v>37811</v>
+      </c>
+      <c r="G21" s="8">
+        <v>368.7</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.00859961</v>
+      </c>
+      <c r="I21" s="9">
         <f t="shared" si="1"/>
-        <v>0.698807542351627</v>
-      </c>
-      <c r="J21" s="6">
-        <v>75064.5</v>
+        <v>1.00368974304523</v>
+      </c>
+      <c r="J21" s="10">
+        <v>29638</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22">
+        <v>33683</v>
+      </c>
+      <c r="C22">
+        <v>95.8</v>
+      </c>
+      <c r="D22" s="2">
+        <v>14112</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B22">
-        <v>37672</v>
-      </c>
-      <c r="C22">
-        <v>355.5</v>
-      </c>
-      <c r="D22" s="2">
-        <v>14967</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22">
-        <v>37269</v>
-      </c>
-      <c r="G22">
-        <v>318.7</v>
-      </c>
-      <c r="H22" s="4">
-        <v>0.00859961</v>
-      </c>
-      <c r="I22" s="5">
+      <c r="F22" s="4">
+        <v>29266</v>
+      </c>
+      <c r="G22" s="4">
+        <v>87.9</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.00839844</v>
+      </c>
+      <c r="I22" s="9">
         <f t="shared" si="1"/>
-        <v>0.989302399660225</v>
-      </c>
-      <c r="J22" s="6">
-        <v>29638</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23">
-        <v>33683</v>
-      </c>
-      <c r="C23">
-        <v>95.8</v>
-      </c>
-      <c r="D23" s="2">
-        <v>14112</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23">
-        <v>28510</v>
-      </c>
-      <c r="G23">
-        <v>71.2</v>
-      </c>
-      <c r="H23" s="4">
-        <v>0.00839844</v>
-      </c>
-      <c r="I23" s="5">
-        <f t="shared" si="1"/>
-        <v>0.846421043256242</v>
-      </c>
-      <c r="J23" s="6">
+        <v>0.868865599857495</v>
+      </c>
+      <c r="J22" s="10">
         <v>5150.52</v>
       </c>
     </row>
-    <row r="24" spans="9:10">
-      <c r="I24" s="5">
-        <f>AVERAGE(I4:I23)</f>
-        <v>0.687836028667346</v>
-      </c>
-      <c r="J24" s="6">
-        <f>AVERAGE(J4:J23)</f>
-        <v>14701.0309952778</v>
+    <row r="23" spans="9:10">
+      <c r="I23" s="9">
+        <f>AVERAGE(I4:I22)</f>
+        <v>0.711602241187247</v>
+      </c>
+      <c r="J23" s="10">
+        <f>AVERAGE(J4:J22)</f>
+        <v>18818.3819955263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test: start test on EPFL under ER<=0.05
</commit_message>
<xml_diff>
--- a/ANS-VECBEE/result/epfl-er.xlsx
+++ b/ANS-VECBEE/result/epfl-er.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
-  <si>
-    <t>er bound = 0.01</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="49">
+  <si>
+    <t>er bound = 0.01, 100000 patterns, use "map -a"</t>
   </si>
   <si>
     <t>circuit</t>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>1001/1</t>
+  </si>
+  <si>
+    <t>er bound = 0.05, 10000 patterns, "use map"</t>
+  </si>
+  <si>
+    <t>delay (from abc)</t>
   </si>
 </sst>
 </file>
@@ -170,7 +176,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +186,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -329,7 +342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,6 +352,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,165 +659,171 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
@@ -811,6 +836,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
@@ -1138,15 +1178,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="14.4" customWidth="true"/>
+    <col min="1" max="1" width="8.5" customWidth="true"/>
     <col min="2" max="2" width="7.3" customWidth="true"/>
     <col min="3" max="3" width="13.4" customWidth="true"/>
     <col min="4" max="4" width="7.3" customWidth="true"/>
@@ -1159,10 +1199,11 @@
     <col min="11" max="11" width="12.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
@@ -1214,10 +1255,10 @@
       <c r="C4">
         <v>303.8</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>1117</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="4">
@@ -1226,14 +1267,14 @@
       <c r="G4" s="4">
         <v>302.6</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="6">
         <v>0</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="16">
         <f t="shared" ref="I4:I10" si="0">F4/B4</f>
         <v>0.968388589051658</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="17">
         <v>3.84195</v>
       </c>
     </row>
@@ -1247,10 +1288,10 @@
       <c r="C5">
         <v>242.6</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>857</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F5">
@@ -1259,14 +1300,14 @@
       <c r="G5">
         <v>64.5</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="7">
         <v>0.00885</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="16">
         <f t="shared" si="0"/>
         <v>0.664816870144284</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="17">
         <v>99.2991</v>
       </c>
     </row>
@@ -1280,26 +1321,26 @@
       <c r="C6">
         <v>51.6</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>1927</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="8">
         <v>5383</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="8">
         <v>51.6</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="6">
         <v>0</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="17">
         <v>6.89306</v>
       </c>
     </row>
@@ -1313,10 +1354,10 @@
       <c r="C7">
         <v>24.2</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>441</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="4">
@@ -1325,14 +1366,14 @@
       <c r="G7" s="4">
         <v>22.5</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="7">
         <v>0.0099</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="16">
         <f t="shared" si="0"/>
         <v>0.978956999085087</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="17">
         <v>6.79064</v>
       </c>
     </row>
@@ -1346,10 +1387,10 @@
       <c r="C8">
         <v>12.7</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>87</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F8">
@@ -1358,14 +1399,14 @@
       <c r="G8">
         <v>11.9</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="7">
         <v>0.00751</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="16">
         <f t="shared" si="0"/>
         <v>0.938461538461538</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="17">
         <v>0.374605</v>
       </c>
     </row>
@@ -1379,10 +1420,10 @@
       <c r="C9">
         <v>29</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>433</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F9">
@@ -1391,14 +1432,14 @@
       <c r="G9">
         <v>15.5</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="7">
         <v>0.00734</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="16">
         <f t="shared" si="0"/>
         <v>0.717587939698492</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="17">
         <v>6.16086</v>
       </c>
     </row>
@@ -1413,10 +1454,10 @@
       <c r="C10">
         <v>5533.8</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="3">
         <v>17710</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F10">
@@ -1425,14 +1466,14 @@
       <c r="G10">
         <v>1668.2</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="7">
         <v>0.00995508</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="16">
         <f t="shared" si="0"/>
         <v>0.21312856811814</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="17">
         <v>92930.7</v>
       </c>
     </row>
@@ -1446,10 +1487,10 @@
       <c r="C11">
         <v>31.2</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>611</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F11">
@@ -1458,14 +1499,14 @@
       <c r="G11">
         <v>31.2</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="7">
         <v>0.00895</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="16">
         <f t="shared" ref="I11:I22" si="1">F11/B11</f>
         <v>0.771708683473389</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="17">
         <v>82.019</v>
       </c>
     </row>
@@ -1479,26 +1520,26 @@
       <c r="C12">
         <v>19.5</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>147</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F12">
         <v>256</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="9">
         <v>18.1</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="7">
         <v>0.00959</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="16">
         <f t="shared" si="1"/>
         <v>0.750733137829912</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="17">
         <v>2.2399</v>
       </c>
     </row>
@@ -1512,10 +1553,10 @@
       <c r="C13">
         <v>651.4</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>27468</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="5" t="s">
         <v>29</v>
       </c>
       <c r="F13" s="4">
@@ -1525,14 +1566,14 @@
       <c r="G13" s="4">
         <v>632.1</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="7">
         <v>0.00952539</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="16">
         <f t="shared" si="1"/>
         <v>0.884427735047641</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="17">
         <v>42595.9</v>
       </c>
     </row>
@@ -1546,10 +1587,10 @@
       <c r="C14">
         <v>466.9</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="2">
         <v>2163</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F14">
@@ -1558,14 +1599,14 @@
       <c r="G14">
         <v>146.7</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="7">
         <v>0.00869</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="16">
         <f t="shared" si="1"/>
         <v>0.471533425907558</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="17">
         <v>526.586</v>
       </c>
     </row>
@@ -1579,10 +1620,10 @@
       <c r="C15">
         <v>101.9</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="3">
         <v>6205</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F15">
@@ -1591,14 +1632,14 @@
       <c r="G15">
         <v>94.5</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="7">
         <v>0.00960156</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="16">
         <f t="shared" si="1"/>
         <v>0.672687615022834</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="17">
         <v>43127.4</v>
       </c>
     </row>
@@ -1606,32 +1647,32 @@
       <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <v>54205</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>419.5</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="3">
         <v>20260</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="8">
         <v>52191</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="10">
         <v>549.9</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="7">
         <v>0.00937793</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="16">
         <f t="shared" si="1"/>
         <v>0.962844756018817</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="17">
         <v>67837.1</v>
       </c>
     </row>
@@ -1645,10 +1686,10 @@
       <c r="C17">
         <v>126.8</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="2">
         <v>351</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="5" t="s">
         <v>36</v>
       </c>
       <c r="F17">
@@ -1657,14 +1698,14 @@
       <c r="G17">
         <v>6.8</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="7">
         <v>0.00382</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="16">
         <f t="shared" si="1"/>
         <v>0.0350877192982456</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="17">
         <v>134.567</v>
       </c>
     </row>
@@ -1678,10 +1719,10 @@
       <c r="C18">
         <v>13.7</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="2">
         <v>109</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F18">
@@ -1690,14 +1731,14 @@
       <c r="G18">
         <v>1.4</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="7">
         <v>0.00627</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="16">
         <f t="shared" si="1"/>
         <v>0.021505376344086</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="17">
         <v>17.1458</v>
       </c>
     </row>
@@ -1711,10 +1752,10 @@
       <c r="C19">
         <v>272.9</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="2">
         <v>5534</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F19" s="4">
@@ -1723,14 +1764,14 @@
       <c r="G19" s="4">
         <v>267.5</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="7">
         <v>0.00979</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="16">
         <f t="shared" si="1"/>
         <v>0.897210743801653</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="17">
         <v>319.22</v>
       </c>
     </row>
@@ -1744,10 +1785,10 @@
       <c r="C20">
         <v>7304</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="3">
         <v>16584</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F20">
@@ -1756,14 +1797,14 @@
       <c r="G20">
         <v>6930</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="7">
         <v>0.00773047</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="16">
         <f t="shared" si="1"/>
         <v>0.698807542351627</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="17">
         <v>75064.5</v>
       </c>
     </row>
@@ -1777,26 +1818,26 @@
       <c r="C21">
         <v>355.5</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="3">
         <v>14967</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="10">
         <v>37811</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="10">
         <v>368.7</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="7">
         <v>0.00859961</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="16">
         <f t="shared" si="1"/>
         <v>1.00368974304523</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="17">
         <v>29638</v>
       </c>
     </row>
@@ -1810,10 +1851,10 @@
       <c r="C22">
         <v>95.8</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="3">
         <v>14112</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="5" t="s">
         <v>46</v>
       </c>
       <c r="F22" s="4">
@@ -1822,28 +1863,661 @@
       <c r="G22" s="4">
         <v>87.9</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="7">
         <v>0.00839844</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="16">
         <f t="shared" si="1"/>
         <v>0.868865599857495</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="17">
         <v>5150.52</v>
       </c>
     </row>
     <row r="23" spans="9:10">
-      <c r="I23" s="9">
+      <c r="I23" s="16">
         <f>AVERAGE(I4:I22)</f>
         <v>0.711602241187247</v>
       </c>
-      <c r="J23" s="10">
+      <c r="J23" s="17">
         <f>AVERAGE(J4:J22)</f>
         <v>18818.3819955263</v>
       </c>
     </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" t="s">
+        <v>8</v>
+      </c>
+      <c r="I28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29">
+        <v>2594</v>
+      </c>
+      <c r="C29">
+        <v>303.8</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1117</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="9">
+        <v>2500</v>
+      </c>
+      <c r="G29" s="9">
+        <f>198.6</f>
+        <v>198.6</v>
+      </c>
+      <c r="H29" s="11">
+        <v>0.03121</v>
+      </c>
+      <c r="I29" s="16">
+        <f t="shared" ref="I29:I47" si="2">F29/B29</f>
+        <v>0.963762528912876</v>
+      </c>
+      <c r="J29" s="17">
+        <v>2.16646</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30">
+        <v>1802</v>
+      </c>
+      <c r="C30">
+        <v>242.6</v>
+      </c>
+      <c r="D30" s="2">
+        <v>857</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="3">
+        <v>1152</v>
+      </c>
+      <c r="G30" s="3">
+        <v>29.7</v>
+      </c>
+      <c r="H30" s="12">
+        <v>0.0370703</v>
+      </c>
+      <c r="I30" s="16">
+        <f t="shared" si="2"/>
+        <v>0.639289678135405</v>
+      </c>
+      <c r="J30" s="17">
+        <v>30.3951</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>5383</v>
+      </c>
+      <c r="C31">
+        <v>51.6</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1927</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="13">
+        <v>5383</v>
+      </c>
+      <c r="G31" s="13">
+        <v>51.6</v>
+      </c>
+      <c r="H31" s="14">
+        <v>0</v>
+      </c>
+      <c r="I31" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J31" s="17">
+        <v>1.33991</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <v>1093</v>
+      </c>
+      <c r="C32">
+        <v>24.2</v>
+      </c>
+      <c r="D32" s="2">
+        <v>441</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="15">
+        <v>989</v>
+      </c>
+      <c r="G32" s="15">
+        <v>10.7</v>
+      </c>
+      <c r="H32" s="12">
+        <v>0.0466143</v>
+      </c>
+      <c r="I32" s="16">
+        <f t="shared" si="2"/>
+        <v>0.904849039341263</v>
+      </c>
+      <c r="J32" s="17">
+        <v>2.56063</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33">
+        <v>195</v>
+      </c>
+      <c r="C33">
+        <v>12.7</v>
+      </c>
+      <c r="D33" s="2">
+        <v>87</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="3">
+        <v>181</v>
+      </c>
+      <c r="G33" s="3">
+        <v>4.9</v>
+      </c>
+      <c r="H33" s="12">
+        <v>0.0309414</v>
+      </c>
+      <c r="I33" s="16">
+        <f t="shared" si="2"/>
+        <v>0.928205128205128</v>
+      </c>
+      <c r="J33" s="17">
+        <v>0.11936</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>995</v>
+      </c>
+      <c r="C34">
+        <v>29</v>
+      </c>
+      <c r="D34" s="2">
+        <v>433</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="3">
+        <v>805</v>
+      </c>
+      <c r="G34" s="3">
+        <v>4.4</v>
+      </c>
+      <c r="H34" s="12">
+        <v>0.0467783</v>
+      </c>
+      <c r="I34" s="16">
+        <f t="shared" si="2"/>
+        <v>0.809045226130653</v>
+      </c>
+      <c r="J34" s="17">
+        <v>6.4459</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35">
+        <f>47469</f>
+        <v>47469</v>
+      </c>
+      <c r="C35">
+        <v>5533.8</v>
+      </c>
+      <c r="D35" s="3">
+        <v>17710</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="17"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36">
+        <v>1428</v>
+      </c>
+      <c r="C36">
+        <v>31.2</v>
+      </c>
+      <c r="D36" s="2">
+        <v>611</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="3">
+        <v>1080</v>
+      </c>
+      <c r="G36" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="H36" s="12">
+        <v>0.0446719</v>
+      </c>
+      <c r="I36" s="16">
+        <f t="shared" si="2"/>
+        <v>0.756302521008403</v>
+      </c>
+      <c r="J36" s="17">
+        <v>21.8659</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37">
+        <v>341</v>
+      </c>
+      <c r="C37">
+        <v>19.5</v>
+      </c>
+      <c r="D37" s="2">
+        <v>147</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="3">
+        <v>232</v>
+      </c>
+      <c r="G37" s="9">
+        <v>8.2</v>
+      </c>
+      <c r="H37" s="12">
+        <v>0.044708</v>
+      </c>
+      <c r="I37" s="16">
+        <f t="shared" si="2"/>
+        <v>0.680351906158358</v>
+      </c>
+      <c r="J37" s="17">
+        <v>0.606447</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38">
+        <v>69688</v>
+      </c>
+      <c r="C38">
+        <v>651.4</v>
+      </c>
+      <c r="D38" s="2">
+        <v>27468</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="17"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39">
+        <v>5041</v>
+      </c>
+      <c r="C39">
+        <v>466.9</v>
+      </c>
+      <c r="D39" s="2">
+        <v>2163</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="3">
+        <v>2456</v>
+      </c>
+      <c r="G39" s="3">
+        <v>18.4</v>
+      </c>
+      <c r="H39" s="12">
+        <v>0.0494697</v>
+      </c>
+      <c r="I39" s="16">
+        <f t="shared" si="2"/>
+        <v>0.487204919658798</v>
+      </c>
+      <c r="J39" s="17">
+        <v>327.801</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40">
+        <v>14671</v>
+      </c>
+      <c r="C40">
+        <v>101.9</v>
+      </c>
+      <c r="D40" s="3">
+        <v>6205</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="17"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="4">
+        <v>54205</v>
+      </c>
+      <c r="C41" s="4">
+        <v>419.5</v>
+      </c>
+      <c r="D41" s="3">
+        <v>20260</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J41" s="17"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42">
+        <v>741</v>
+      </c>
+      <c r="C42">
+        <v>126.8</v>
+      </c>
+      <c r="D42" s="2">
+        <v>351</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F42" s="3">
+        <v>15</v>
+      </c>
+      <c r="G42" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="H42" s="12">
+        <v>0.046833</v>
+      </c>
+      <c r="I42" s="16">
+        <f t="shared" si="2"/>
+        <v>0.0202429149797571</v>
+      </c>
+      <c r="J42" s="17">
+        <v>16.7512</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43">
+        <v>186</v>
+      </c>
+      <c r="C43">
+        <v>13.7</v>
+      </c>
+      <c r="D43" s="2">
+        <v>109</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="3">
+        <v>4</v>
+      </c>
+      <c r="G43" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="H43" s="12">
+        <v>0.00605273</v>
+      </c>
+      <c r="I43" s="16">
+        <f t="shared" si="2"/>
+        <v>0.021505376344086</v>
+      </c>
+      <c r="J43" s="17">
+        <v>2.9771</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44">
+        <v>13552</v>
+      </c>
+      <c r="C44">
+        <v>272.9</v>
+      </c>
+      <c r="D44" s="2">
+        <v>5534</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F44" s="15">
+        <v>12825</v>
+      </c>
+      <c r="G44" s="15">
+        <v>117.9</v>
+      </c>
+      <c r="H44" s="12">
+        <v>0.0452158</v>
+      </c>
+      <c r="I44" s="16">
+        <f t="shared" si="2"/>
+        <v>0.946354781582054</v>
+      </c>
+      <c r="J44" s="17">
+        <v>158.788</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45">
+        <v>43859</v>
+      </c>
+      <c r="C45">
+        <v>7304</v>
+      </c>
+      <c r="D45" s="3">
+        <v>16584</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J45" s="17"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46">
+        <v>37672</v>
+      </c>
+      <c r="C46">
+        <v>355.5</v>
+      </c>
+      <c r="D46" s="3">
+        <v>14967</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J46" s="17"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>33683</v>
+      </c>
+      <c r="C47">
+        <v>95.8</v>
+      </c>
+      <c r="D47" s="3">
+        <v>14112</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J47" s="17"/>
+    </row>
+    <row r="48" spans="6:10">
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="16">
+        <f>AVERAGE(I29:I47)</f>
+        <v>0.429321790550357</v>
+      </c>
+      <c r="J48" s="17"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A26:B26"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
test: some experiments on EPFL with ER of 0.05
</commit_message>
<xml_diff>
--- a/ANS-VECBEE/result/epfl-er.xlsx
+++ b/ANS-VECBEE/result/epfl-er.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="49">
   <si>
-    <t>er bound = 0.01, 100000 patterns, use "map -a"</t>
+    <t>er bound = 0.01, 100000 patterns</t>
   </si>
   <si>
     <t>circuit</t>
@@ -157,7 +157,7 @@
     <t>1001/1</t>
   </si>
   <si>
-    <t>er bound = 0.05, 10000 patterns, "use map"</t>
+    <t>er bound = 0.05, 10000 patterns</t>
   </si>
   <si>
     <t>delay (from abc)</t>
@@ -168,13 +168,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="0.0_ "/>
-    <numFmt numFmtId="177" formatCode="0.000_ "/>
-    <numFmt numFmtId="178" formatCode="0.0000_ "/>
+    <numFmt numFmtId="176" formatCode="0.000_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="0.0_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -198,8 +198,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,7 +208,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,16 +222,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,9 +245,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,15 +261,60 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -284,30 +329,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,30 +341,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,7 +357,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -369,7 +459,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,169 +495,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,17 +551,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -584,8 +574,32 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -606,21 +620,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -635,22 +634,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -659,109 +653,109 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
@@ -770,41 +764,41 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -814,49 +808,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1180,8 +1168,8 @@
   <sheetPr/>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>
@@ -1258,23 +1246,23 @@
       <c r="D4" s="2">
         <v>1117</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>2512</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>302.6</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>0</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="14">
         <f t="shared" ref="I4:I10" si="0">F4/B4</f>
         <v>0.968388589051658</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="15">
         <v>3.84195</v>
       </c>
     </row>
@@ -1291,7 +1279,7 @@
       <c r="D5" s="2">
         <v>857</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F5">
@@ -1300,14 +1288,14 @@
       <c r="G5">
         <v>64.5</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <v>0.00885</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="14">
         <f t="shared" si="0"/>
         <v>0.664816870144284</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="15">
         <v>99.2991</v>
       </c>
     </row>
@@ -1324,23 +1312,23 @@
       <c r="D6" s="2">
         <v>1927</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>5383</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>51.6</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>0</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="14">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="15">
         <v>6.89306</v>
       </c>
     </row>
@@ -1357,23 +1345,23 @@
       <c r="D7" s="2">
         <v>441</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>1070</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>22.5</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>0.0099</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="14">
         <f t="shared" si="0"/>
         <v>0.978956999085087</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="15">
         <v>6.79064</v>
       </c>
     </row>
@@ -1390,7 +1378,7 @@
       <c r="D8" s="2">
         <v>87</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F8">
@@ -1399,14 +1387,14 @@
       <c r="G8">
         <v>11.9</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>0.00751</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="14">
         <f t="shared" si="0"/>
         <v>0.938461538461538</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="15">
         <v>0.374605</v>
       </c>
     </row>
@@ -1423,7 +1411,7 @@
       <c r="D9" s="2">
         <v>433</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F9">
@@ -1432,14 +1420,14 @@
       <c r="G9">
         <v>15.5</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <v>0.00734</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="14">
         <f t="shared" si="0"/>
         <v>0.717587939698492</v>
       </c>
-      <c r="J9" s="17">
+      <c r="J9" s="15">
         <v>6.16086</v>
       </c>
     </row>
@@ -1454,10 +1442,10 @@
       <c r="C10">
         <v>5533.8</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>17710</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F10">
@@ -1466,14 +1454,14 @@
       <c r="G10">
         <v>1668.2</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>0.00995508</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="14">
         <f t="shared" si="0"/>
         <v>0.21312856811814</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="15">
         <v>92930.7</v>
       </c>
     </row>
@@ -1490,7 +1478,7 @@
       <c r="D11" s="2">
         <v>611</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F11">
@@ -1499,14 +1487,14 @@
       <c r="G11">
         <v>31.2</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>0.00895</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="14">
         <f t="shared" ref="I11:I22" si="1">F11/B11</f>
         <v>0.771708683473389</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="15">
         <v>82.019</v>
       </c>
     </row>
@@ -1523,23 +1511,23 @@
       <c r="D12" s="2">
         <v>147</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F12">
         <v>256</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>18.1</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>0.00959</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="14">
         <f t="shared" si="1"/>
         <v>0.750733137829912</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="15">
         <v>2.2399</v>
       </c>
     </row>
@@ -1556,24 +1544,24 @@
       <c r="D13" s="2">
         <v>27468</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <f>61634</f>
         <v>61634</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>632.1</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <v>0.00952539</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="14">
         <f t="shared" si="1"/>
         <v>0.884427735047641</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13" s="15">
         <v>42595.9</v>
       </c>
     </row>
@@ -1590,7 +1578,7 @@
       <c r="D14" s="2">
         <v>2163</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F14">
@@ -1599,14 +1587,14 @@
       <c r="G14">
         <v>146.7</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="6">
         <v>0.00869</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="14">
         <f t="shared" si="1"/>
         <v>0.471533425907558</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J14" s="15">
         <v>526.586</v>
       </c>
     </row>
@@ -1620,10 +1608,10 @@
       <c r="C15">
         <v>101.9</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>6205</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>33</v>
       </c>
       <c r="F15">
@@ -1632,14 +1620,14 @@
       <c r="G15">
         <v>94.5</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="6">
         <v>0.00960156</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="14">
         <f t="shared" si="1"/>
         <v>0.672687615022834</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J15" s="15">
         <v>43127.4</v>
       </c>
     </row>
@@ -1647,32 +1635,32 @@
       <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>54205</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>419.5</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>20260</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="7">
         <v>52191</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="9">
         <v>549.9</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="6">
         <v>0.00937793</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="14">
         <f t="shared" si="1"/>
         <v>0.962844756018817</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J16" s="15">
         <v>67837.1</v>
       </c>
     </row>
@@ -1689,7 +1677,7 @@
       <c r="D17" s="2">
         <v>351</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F17">
@@ -1698,14 +1686,14 @@
       <c r="G17">
         <v>6.8</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="6">
         <v>0.00382</v>
       </c>
-      <c r="I17" s="16">
+      <c r="I17" s="14">
         <f t="shared" si="1"/>
         <v>0.0350877192982456</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="15">
         <v>134.567</v>
       </c>
     </row>
@@ -1722,7 +1710,7 @@
       <c r="D18" s="2">
         <v>109</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F18">
@@ -1731,14 +1719,14 @@
       <c r="G18">
         <v>1.4</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="6">
         <v>0.00627</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="14">
         <f t="shared" si="1"/>
         <v>0.021505376344086</v>
       </c>
-      <c r="J18" s="17">
+      <c r="J18" s="15">
         <v>17.1458</v>
       </c>
     </row>
@@ -1755,23 +1743,23 @@
       <c r="D19" s="2">
         <v>5534</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <v>12159</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>267.5</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="6">
         <v>0.00979</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I19" s="14">
         <f t="shared" si="1"/>
         <v>0.897210743801653</v>
       </c>
-      <c r="J19" s="17">
+      <c r="J19" s="15">
         <v>319.22</v>
       </c>
     </row>
@@ -1785,10 +1773,10 @@
       <c r="C20">
         <v>7304</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>16584</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>42</v>
       </c>
       <c r="F20">
@@ -1797,14 +1785,14 @@
       <c r="G20">
         <v>6930</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="6">
         <v>0.00773047</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="14">
         <f t="shared" si="1"/>
         <v>0.698807542351627</v>
       </c>
-      <c r="J20" s="17">
+      <c r="J20" s="15">
         <v>75064.5</v>
       </c>
     </row>
@@ -1818,26 +1806,26 @@
       <c r="C21">
         <v>355.5</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>14967</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="9">
         <v>37811</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="9">
         <v>368.7</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="6">
         <v>0.00859961</v>
       </c>
-      <c r="I21" s="16">
+      <c r="I21" s="14">
         <f t="shared" si="1"/>
         <v>1.00368974304523</v>
       </c>
-      <c r="J21" s="17">
+      <c r="J21" s="15">
         <v>29638</v>
       </c>
     </row>
@@ -1851,35 +1839,35 @@
       <c r="C22">
         <v>95.8</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>14112</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <v>29266</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <v>87.9</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="6">
         <v>0.00839844</v>
       </c>
-      <c r="I22" s="16">
+      <c r="I22" s="14">
         <f t="shared" si="1"/>
         <v>0.868865599857495</v>
       </c>
-      <c r="J22" s="17">
+      <c r="J22" s="15">
         <v>5150.52</v>
       </c>
     </row>
     <row r="23" spans="9:10">
-      <c r="I23" s="16">
+      <c r="I23" s="14">
         <f>AVERAGE(I4:I22)</f>
         <v>0.711602241187247</v>
       </c>
-      <c r="J23" s="17">
+      <c r="J23" s="15">
         <f>AVERAGE(J4:J22)</f>
         <v>18818.3819955263</v>
       </c>
@@ -1943,26 +1931,17 @@
       <c r="D29" s="2">
         <v>1117</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="9">
-        <v>2500</v>
-      </c>
-      <c r="G29" s="9">
-        <f>198.6</f>
-        <v>198.6</v>
-      </c>
-      <c r="H29" s="11">
-        <v>0.03121</v>
-      </c>
-      <c r="I29" s="16">
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="14">
         <f t="shared" ref="I29:I47" si="2">F29/B29</f>
-        <v>0.963762528912876</v>
-      </c>
-      <c r="J29" s="17">
-        <v>2.16646</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J29" s="15"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
@@ -1977,25 +1956,17 @@
       <c r="D30" s="2">
         <v>857</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="3">
-        <v>1152</v>
-      </c>
-      <c r="G30" s="3">
-        <v>29.7</v>
-      </c>
-      <c r="H30" s="12">
-        <v>0.0370703</v>
-      </c>
-      <c r="I30" s="16">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="14">
         <f t="shared" si="2"/>
-        <v>0.639289678135405</v>
-      </c>
-      <c r="J30" s="17">
-        <v>30.3951</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J30" s="15"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
@@ -2010,25 +1981,17 @@
       <c r="D31" s="2">
         <v>1927</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="13">
-        <v>5383</v>
-      </c>
-      <c r="G31" s="13">
-        <v>51.6</v>
-      </c>
-      <c r="H31" s="14">
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="14">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I31" s="16">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J31" s="17">
-        <v>1.33991</v>
-      </c>
+      <c r="J31" s="15"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
@@ -2043,25 +2006,17 @@
       <c r="D32" s="2">
         <v>441</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="15">
-        <v>989</v>
-      </c>
-      <c r="G32" s="15">
-        <v>10.7</v>
-      </c>
-      <c r="H32" s="12">
-        <v>0.0466143</v>
-      </c>
-      <c r="I32" s="16">
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="14">
         <f t="shared" si="2"/>
-        <v>0.904849039341263</v>
-      </c>
-      <c r="J32" s="17">
-        <v>2.56063</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J32" s="15"/>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
@@ -2076,25 +2031,17 @@
       <c r="D33" s="2">
         <v>87</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="3">
-        <v>181</v>
-      </c>
-      <c r="G33" s="3">
-        <v>4.9</v>
-      </c>
-      <c r="H33" s="12">
-        <v>0.0309414</v>
-      </c>
-      <c r="I33" s="16">
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="14">
         <f t="shared" si="2"/>
-        <v>0.928205128205128</v>
-      </c>
-      <c r="J33" s="17">
-        <v>0.11936</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J33" s="15"/>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
@@ -2109,25 +2056,17 @@
       <c r="D34" s="2">
         <v>433</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F34" s="3">
-        <v>805</v>
-      </c>
-      <c r="G34" s="3">
-        <v>4.4</v>
-      </c>
-      <c r="H34" s="12">
-        <v>0.0467783</v>
-      </c>
-      <c r="I34" s="16">
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="14">
         <f t="shared" si="2"/>
-        <v>0.809045226130653</v>
-      </c>
-      <c r="J34" s="17">
-        <v>6.4459</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J34" s="15"/>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
@@ -2140,20 +2079,20 @@
       <c r="C35">
         <v>5533.8</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="2">
         <v>17710</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="16">
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J35" s="17"/>
+      <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
@@ -2168,25 +2107,17 @@
       <c r="D36" s="2">
         <v>611</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F36" s="3">
-        <v>1080</v>
-      </c>
-      <c r="G36" s="3">
-        <v>9.5</v>
-      </c>
-      <c r="H36" s="12">
-        <v>0.0446719</v>
-      </c>
-      <c r="I36" s="16">
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="14">
         <f t="shared" si="2"/>
-        <v>0.756302521008403</v>
-      </c>
-      <c r="J36" s="17">
-        <v>21.8659</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
@@ -2201,25 +2132,17 @@
       <c r="D37" s="2">
         <v>147</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F37" s="3">
-        <v>232</v>
-      </c>
-      <c r="G37" s="9">
-        <v>8.2</v>
-      </c>
-      <c r="H37" s="12">
-        <v>0.044708</v>
-      </c>
-      <c r="I37" s="16">
+      <c r="F37" s="2"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="14">
         <f t="shared" si="2"/>
-        <v>0.680351906158358</v>
-      </c>
-      <c r="J37" s="17">
-        <v>0.606447</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
@@ -2234,17 +2157,17 @@
       <c r="D38" s="2">
         <v>27468</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="16">
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J38" s="17"/>
+      <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
@@ -2259,25 +2182,17 @@
       <c r="D39" s="2">
         <v>2163</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F39" s="3">
-        <v>2456</v>
-      </c>
-      <c r="G39" s="3">
-        <v>18.4</v>
-      </c>
-      <c r="H39" s="12">
-        <v>0.0494697</v>
-      </c>
-      <c r="I39" s="16">
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="14">
         <f t="shared" si="2"/>
-        <v>0.487204919658798</v>
-      </c>
-      <c r="J39" s="17">
-        <v>327.801</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J39" s="15"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
@@ -2289,45 +2204,45 @@
       <c r="C40">
         <v>101.9</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <v>6205</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="16">
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J40" s="17"/>
+      <c r="J40" s="15"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>34</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="3">
         <v>54205</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="3">
         <v>419.5</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="2">
         <v>20260</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F41" s="2"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="16">
+      <c r="G41" s="8"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J41" s="17"/>
+      <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
@@ -2342,25 +2257,17 @@
       <c r="D42" s="2">
         <v>351</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F42" s="3">
-        <v>15</v>
-      </c>
-      <c r="G42" s="3">
-        <v>2.9</v>
-      </c>
-      <c r="H42" s="12">
-        <v>0.046833</v>
-      </c>
-      <c r="I42" s="16">
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="14">
         <f t="shared" si="2"/>
-        <v>0.0202429149797571</v>
-      </c>
-      <c r="J42" s="17">
-        <v>16.7512</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J42" s="15"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
@@ -2375,25 +2282,17 @@
       <c r="D43" s="2">
         <v>109</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F43" s="3">
-        <v>4</v>
-      </c>
-      <c r="G43" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="H43" s="12">
-        <v>0.00605273</v>
-      </c>
-      <c r="I43" s="16">
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="14">
         <f t="shared" si="2"/>
-        <v>0.021505376344086</v>
-      </c>
-      <c r="J43" s="17">
-        <v>2.9771</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J43" s="15"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
@@ -2408,25 +2307,17 @@
       <c r="D44" s="2">
         <v>5534</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E44" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F44" s="15">
-        <v>12825</v>
-      </c>
-      <c r="G44" s="15">
-        <v>117.9</v>
-      </c>
-      <c r="H44" s="12">
-        <v>0.0452158</v>
-      </c>
-      <c r="I44" s="16">
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="14">
         <f t="shared" si="2"/>
-        <v>0.946354781582054</v>
-      </c>
-      <c r="J44" s="17">
-        <v>158.788</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J44" s="15"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
@@ -2438,20 +2329,20 @@
       <c r="C45">
         <v>7304</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="2">
         <v>16584</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="16">
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J45" s="17"/>
+      <c r="J45" s="15"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
@@ -2463,20 +2354,20 @@
       <c r="C46">
         <v>355.5</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="2">
         <v>14967</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="16">
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J46" s="17"/>
+      <c r="J46" s="15"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
@@ -2488,30 +2379,30 @@
       <c r="C47">
         <v>95.8</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="2">
         <v>14112</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="16">
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J47" s="17"/>
+      <c r="J47" s="15"/>
     </row>
     <row r="48" spans="6:10">
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="16">
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="14">
         <f>AVERAGE(I29:I47)</f>
-        <v>0.429321790550357</v>
-      </c>
-      <c r="J48" s="17"/>
+        <v>0</v>
+      </c>
+      <c r="J48" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>